<commit_message>
Made updates according to review comments and remarks Deleted AdministrationPage class, deleted changes for default DataGather files, changed VIN number for Choice product tests
</commit_message>
<xml_diff>
--- a/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/VINupload_CA_CHOICE_UPDATE.xlsx
+++ b/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/VINupload_CA_CHOICE_UPDATE.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="51">
   <si>
     <t>VIN</t>
   </si>
@@ -116,64 +116,67 @@
     <t>ALTFUEL</t>
   </si>
   <si>
+    <t>TEST</t>
+  </si>
+  <si>
+    <t>SYMBOL_2000_CHOICE</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>SYMBOL_2000_CHOICE_T</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>4T1BE30K&amp;6</t>
+  </si>
+  <si>
+    <t>TOYT</t>
+  </si>
+  <si>
+    <t>TOYOTA</t>
+  </si>
+  <si>
+    <t>CAMRY</t>
+  </si>
+  <si>
+    <t>CAMRY LE/XLE/SE</t>
+  </si>
+  <si>
+    <t>4D SED</t>
+  </si>
+  <si>
+    <t>SEDAN 4 DOOR</t>
+  </si>
+  <si>
+    <t>SED</t>
+  </si>
+  <si>
+    <t>2.4L L4</t>
+  </si>
+  <si>
     <t>2WD</t>
   </si>
   <si>
+    <t>000S</t>
+  </si>
+  <si>
+    <t>FRONT, HEAD &amp; SIDE AIRBAGS</t>
+  </si>
+  <si>
+    <t>4 WHEEL STANDARD</t>
+  </si>
+  <si>
     <t>STD</t>
   </si>
   <si>
-    <t>1HGEM215&amp;4</t>
-  </si>
-  <si>
-    <t>TEST</t>
-  </si>
-  <si>
-    <t>SYMBOL_2000_CHOICE</t>
-  </si>
-  <si>
-    <t>HOND</t>
-  </si>
-  <si>
-    <t>HONDA</t>
-  </si>
-  <si>
-    <t>CIVIC</t>
-  </si>
-  <si>
-    <t>CIVIC LX</t>
-  </si>
-  <si>
-    <t>2D CPE</t>
-  </si>
-  <si>
-    <t>COUPE</t>
-  </si>
-  <si>
-    <t>CPE</t>
-  </si>
-  <si>
-    <t>1.7L L4</t>
-  </si>
-  <si>
-    <t>000E</t>
-  </si>
-  <si>
-    <t>FRONT AIRBAGS</t>
-  </si>
-  <si>
-    <t>NOT AVAILABLE</t>
-  </si>
-  <si>
-    <t>P-PASSIVE SENTRY KEY</t>
+    <t>H-IMMOBILIZER/ALARM</t>
   </si>
   <si>
     <t>I</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>SYMBOL_2000_CHOICE_T</t>
   </si>
 </sst>
 </file>
@@ -522,8 +525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
+      <selection activeCell="AA15" sqref="AA15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -648,42 +651,42 @@
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C2" s="4">
-        <v>2004</v>
+        <v>2006</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H2" s="4">
         <v>20000</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="K2" s="4"/>
       <c r="L2" s="4"/>
       <c r="M2" s="4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="O2" s="4">
         <v>4</v>
@@ -691,87 +694,87 @@
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
       <c r="R2" s="4" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="S2" s="4">
         <v>2</v>
       </c>
       <c r="T2" s="4" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="U2" s="4" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="V2" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="W2" s="4" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="X2" s="4" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="Y2" s="4" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="Z2" s="4" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="AA2" s="4">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="AB2" s="4">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="AC2" s="4" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="AD2" s="4" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="C3" s="4">
-        <v>2004</v>
+        <v>2006</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="H3" s="4">
         <v>20000</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="O3" s="4">
         <v>4</v>
@@ -779,43 +782,43 @@
       <c r="P3" s="4"/>
       <c r="Q3" s="4"/>
       <c r="R3" s="4" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="S3" s="4">
         <v>2</v>
       </c>
       <c r="T3" s="4" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="U3" s="4" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="V3" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="W3" s="4" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="X3" s="4" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="Y3" s="4" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="Z3" s="4" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="AA3" s="4">
-        <v>44</v>
+        <v>12</v>
       </c>
       <c r="AB3" s="4">
-        <v>44</v>
+        <v>13</v>
       </c>
       <c r="AC3" s="4" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="AD3" s="4" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.3">

</xml_diff>